<commit_message>
updates to Array and Linked List Features
updates to Array and Linked List Features
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya Yelakala\eclipse-workspace\DSAlgo_TeamAchievers\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D16A0C5-0006-4D51-A537-DD7F00EDBC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FAEE00-1A6F-4E42-9D51-B784C55676B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
     <sheet name="pythonCode1" sheetId="4" r:id="rId5"/>
     <sheet name="tryEditorCode" sheetId="7" r:id="rId6"/>
+    <sheet name="ArrayPracticeQnsQ1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>username</t>
   </si>
@@ -347,6 +348,14 @@
   </si>
   <si>
     <t>gdfgdgdfhdhd</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+    if num in input_list:
+        print("Element Found")
+    else:
+        print("Not Found")
+search([12, 23, 45, 67, 6, 90], 12)</t>
   </si>
 </sst>
 </file>
@@ -451,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -480,6 +489,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1391,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF521D5E-4550-427D-AF53-CC1823D613EE}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1418,4 +1430,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273A76BE-57E6-4F96-99B3-513903090E7F}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="100.8">
+      <c r="A2" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="172.8">
+      <c r="A3" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Array and DS features
updated Array and DS features
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya Yelakala\eclipse-workspace\DSAlgo_TeamAchievers\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FAEE00-1A6F-4E42-9D51-B784C55676B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F236BAE7-3DA9-4F43-BBBD-CBC1CD7CF736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="2" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF521D5E-4550-427D-AF53-CC1823D613EE}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1436,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273A76BE-57E6-4F96-99B3-513903090E7F}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>

</xml_diff>